<commit_message>
changed profile pic path
</commit_message>
<xml_diff>
--- a/OrangeHRMTest/src/test/resources/testdata/testdata.xlsx
+++ b/OrangeHRMTest/src/test/resources/testdata/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhivy\eclipse-workspace\OrangeHRMTest\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhivy\git\dhivyabharathi-ns\dhivyabharathi-ns\OrangeHRMTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0C04BA-CDBC-4496-879A-7E16B7C3416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AAE4E7-82CC-4009-BC05-44B7E913CBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="666" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginPositive" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F62BB7-59BD-4143-BEF7-FBFFFAD3A50B}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update dashboard and screenshot
</commit_message>
<xml_diff>
--- a/OrangeHRMTest/src/test/resources/testdata/testdata.xlsx
+++ b/OrangeHRMTest/src/test/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhivy\git\dhivyabharathi-ns\dhivyabharathi-ns\OrangeHRMTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA530450-B856-4DB9-9E18-F27D73185CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49739891-A712-4C9F-AEEA-6FCAB631DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,7 +672,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>